<commit_message>
se actualiza formulas para calculo de dias
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Vacaciones_keytronics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBC0DC2-F14C-4108-81A2-2BB618473270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A180F8D-D70E-4A20-9D26-96D7C563F5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2017387C-E726-409B-B94E-7E99E2D436B1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -54,9 +54,6 @@
     <t>area</t>
   </si>
   <si>
-    <t>dias_vacaciones</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -412,6 +409,18 @@
   </si>
   <si>
     <t>jlunaa@keytronics.com</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>correo_notificaciones</t>
+  </si>
+  <si>
+    <t>id_responsable</t>
+  </si>
+  <si>
+    <t>activo</t>
   </si>
 </sst>
 </file>
@@ -456,9 +465,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -774,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D3138F-A59F-4455-A300-0E09E802E78B}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,7 +797,7 @@
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -807,787 +817,913 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="2">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G9" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G10" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G13" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="G17" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G18" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G23" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G24" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G25" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G26" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G27" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G28" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G29" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G30" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31">
         <v>123456</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G31" s="2">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D32">
         <v>123456</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G32" s="2">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33">
         <v>123456</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G33" s="2">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G34" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G35" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G36" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G37" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G38" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="G39" s="2">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="G40" s="2">
+        <v>45658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de la tabla de usuarios
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Vacaciones_keytronics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126D343F-61B6-49F4-B895-EDF1008D1278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DBD7BA-DA59-46EC-876F-E7FC70D5DD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2017387C-E726-409B-B94E-7E99E2D436B1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
   <si>
     <t>id</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>acampo@keytronics.com</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Humberto</t>
+  </si>
+  <si>
+    <t>correo@prueba.com</t>
   </si>
 </sst>
 </file>
@@ -790,7 +799,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,6 +863,15 @@
       <c r="G2" s="2">
         <v>45292</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1732,8 +1750,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C32" r:id="rId1" xr:uid="{CC007ADD-1529-470E-B90E-F900F5D05F68}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{0D8D4B43-1EB0-496A-B7C4-4842697D1712}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>